<commit_message>
Modifiche pre trailer 2
</commit_message>
<xml_diff>
--- a/Piano_Caricamento_Instagram.xlsx
+++ b/Piano_Caricamento_Instagram.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Desktop\gta IV\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE202D3F-BE06-4D4B-98BB-5363CE0B4935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="37">
   <si>
     <t>Settimana</t>
   </si>
@@ -49,12 +55,6 @@
     <t>2024-10-30</t>
   </si>
   <si>
-    <t>2024-10-31</t>
-  </si>
-  <si>
-    <t>2024-11-05</t>
-  </si>
-  <si>
     <t>2024-11-06</t>
   </si>
   <si>
@@ -109,35 +109,35 @@
     <t>Post interattivo (es. domanda al pubblico o sondaggio nelle storie)</t>
   </si>
   <si>
-    <t>Collaborazione o contenuto user-generated</t>
-  </si>
-  <si>
     <t>Reel con tutorial o spiegazione di un argomento rilevante</t>
   </si>
   <si>
-    <t>Infografica o carosello educativo</t>
-  </si>
-  <si>
-    <t>Testimonianza o caso studio</t>
-  </si>
-  <si>
     <t>Reel di intrattenimento (es. tendenze o meme del settore)</t>
   </si>
   <si>
-    <t>Post riassuntivo o highlights del mese</t>
-  </si>
-  <si>
-    <t>Feedback o ringraziamento al pubblico</t>
-  </si>
-  <si>
-    <t>Carosello riepilogativo con statistiche o novità finali</t>
+    <t>pubblicato</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>si</t>
+  </si>
+  <si>
+    <t>Reel con spiegazione</t>
+  </si>
+  <si>
+    <t>immagine</t>
+  </si>
+  <si>
+    <t>reel con spiegazione</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -153,6 +153,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -162,7 +170,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -185,28 +193,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -244,7 +276,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -278,6 +310,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -312,9 +345,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -487,14 +521,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -510,8 +552,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -519,16 +564,19 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -536,186 +584,196 @@
         <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
+      <c r="B4" s="2">
+        <v>45596</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>27</v>
+      </c>
+      <c r="F4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
-        <v>12</v>
+      <c r="B5" s="2">
+        <v>45598</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>28</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>22</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" t="s">
-        <v>38</v>
+        <v>24</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>